<commit_message>
feat: lab id added
</commit_message>
<xml_diff>
--- a/real_data/Fasit_kres_eu.xlsx
+++ b/real_data/Fasit_kres_eu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayoung\Desktop\Thesis\real_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923A426D-E26D-418A-9DC7-4B962467653B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20707D28-9209-45BF-8DF6-97F4FA2097E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8335" yWindow="2270" windowWidth="21600" windowHeight="10900" xr2:uid="{69898852-D492-4A31-81A3-EC70B8AD3B90}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{69898852-D492-4A31-81A3-EC70B8AD3B90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: fixed value range
</commit_message>
<xml_diff>
--- a/real_data/Fasit_kres_eu.xlsx
+++ b/real_data/Fasit_kres_eu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayoung\Desktop\Thesis\real_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20707D28-9209-45BF-8DF6-97F4FA2097E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067446CF-8185-46ED-B75E-EFFD164A67C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{69898852-D492-4A31-81A3-EC70B8AD3B90}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="15600" xr2:uid="{69898852-D492-4A31-81A3-EC70B8AD3B90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Avlesning K-res</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>correct</t>
+  </si>
+  <si>
+    <t>reference MIC</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +107,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,7 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,6 +162,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,14 +493,15 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="3" width="19.42578125" style="4" customWidth="1"/>
-    <col min="4" max="5" width="19.42578125" style="4"/>
+    <col min="4" max="4" width="19.42578125" style="4"/>
+    <col min="5" max="5" width="19.42578125" style="7"/>
     <col min="6" max="6" width="19.42578125"/>
   </cols>
   <sheetData>
@@ -486,12 +509,14 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -505,7 +530,7 @@
       <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -522,7 +547,7 @@
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -542,7 +567,7 @@
       <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="7">
         <v>128</v>
       </c>
       <c r="F5" s="4">
@@ -562,7 +587,7 @@
       <c r="D6" s="4">
         <v>256</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="7">
         <v>64</v>
       </c>
       <c r="F6" s="4">
@@ -582,7 +607,7 @@
       <c r="D7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="7">
         <v>64</v>
       </c>
       <c r="F7" s="4">
@@ -602,7 +627,7 @@
       <c r="D8" s="4">
         <v>4</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="7">
         <v>1</v>
       </c>
       <c r="F8" s="4">
@@ -622,7 +647,7 @@
       <c r="D9" s="4">
         <v>64</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="7">
         <v>16</v>
       </c>
       <c r="F9" s="4">
@@ -642,7 +667,7 @@
       <c r="D10" s="4">
         <v>2</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="7">
         <v>1</v>
       </c>
       <c r="F10" s="4">
@@ -662,7 +687,7 @@
       <c r="D11" s="4">
         <v>16</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="7">
         <v>8</v>
       </c>
       <c r="F11" s="4">
@@ -682,7 +707,7 @@
       <c r="D12" s="4">
         <v>8</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="7">
         <v>2</v>
       </c>
       <c r="F12" s="4">
@@ -702,7 +727,7 @@
       <c r="D13" s="4">
         <v>16</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="7">
         <v>8</v>
       </c>
       <c r="F13" s="4">
@@ -722,7 +747,7 @@
       <c r="D14" s="4">
         <v>16</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="7">
         <v>8</v>
       </c>
       <c r="F14" s="4">
@@ -742,7 +767,7 @@
       <c r="D15" s="4">
         <v>128</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="7">
         <v>64</v>
       </c>
       <c r="F15" s="4">
@@ -762,7 +787,7 @@
       <c r="D16" s="4">
         <v>32</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="7">
         <v>16</v>
       </c>
       <c r="F16" s="4">
@@ -782,7 +807,7 @@
       <c r="D17" s="4">
         <v>64</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="7">
         <v>16</v>
       </c>
       <c r="F17" s="4">
@@ -802,7 +827,7 @@
       <c r="D18" s="4">
         <v>32</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="7">
         <v>8</v>
       </c>
       <c r="F18" s="4">
@@ -822,7 +847,7 @@
       <c r="D19" s="4">
         <v>4</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="7">
         <v>2</v>
       </c>
       <c r="F19" s="4">
@@ -842,7 +867,7 @@
       <c r="D20" s="4">
         <v>32</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="7">
         <v>16</v>
       </c>
       <c r="F20" s="4">
@@ -862,7 +887,7 @@
       <c r="D21" s="4">
         <v>4</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="7">
         <v>2</v>
       </c>
       <c r="F21" s="4">
@@ -882,7 +907,7 @@
       <c r="D22" s="4">
         <v>32</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="7">
         <v>8</v>
       </c>
       <c r="F22" s="4">
@@ -902,7 +927,7 @@
       <c r="D23" s="4">
         <v>4</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="7">
         <v>2</v>
       </c>
       <c r="F23" s="4">
@@ -922,7 +947,7 @@
       <c r="D24" s="4">
         <v>4</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="7">
         <v>4</v>
       </c>
       <c r="F24" s="4">
@@ -939,7 +964,7 @@
       <c r="D25" s="4">
         <v>8</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="7">
         <v>2</v>
       </c>
       <c r="F25" s="4">
@@ -956,7 +981,7 @@
       <c r="D26" s="4">
         <v>4</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="7">
         <v>2</v>
       </c>
       <c r="F26" s="4">
@@ -965,41 +990,41 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27"/>
-      <c r="E27"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
-      <c r="E29"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30"/>
       <c r="C30"/>
-      <c r="E30"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31"/>
       <c r="C31"/>
-      <c r="E31"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32"/>
       <c r="C32"/>
-      <c r="E32"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33"/>
       <c r="C33"/>
-      <c r="E33"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34"/>
       <c r="C34"/>
-      <c r="E34"/>
+      <c r="E34" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>